<commit_message>
update Hyp, add flowchart documents
</commit_message>
<xml_diff>
--- a/Data sets/Hyp/inclusion_Hyp.xlsx
+++ b/Data sets/Hyp/inclusion_Hyp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EliseSchramkowski\Documents\GitHub\thesis\Data sets\Hyp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC065884-52DD-4283-AFD7-0DDFBC9020DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241932ED-6BDB-47E1-ACFA-F0B1A2DB9C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13512" yWindow="2952" windowWidth="15120" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Articles" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="657">
   <si>
     <t>Journal</t>
   </si>
@@ -2053,12 +2053,15 @@
   <si>
     <t>P-values were reported as z-intervals, e.g., as 1.96 &lt; z &lt; 1.64. Since these intervals make it really unclear what p-values were assigned to what results, we decided to exclude results based on these intervals: it is imperative that some sort of p-value is reported, and reporting only z-intervals is therefore not sufficient for an article to be included.</t>
   </si>
+  <si>
+    <t>Relevant statistics not related to explicitly stated hypothesis</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2089,13 +2092,6 @@
     <font>
       <sz val="11"/>
       <color theme="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2155,24 +2151,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="204">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2180,7 +2175,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2338,7 +2332,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2365,7 +2359,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2682,8 +2676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M325"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="K93" sqref="K93"/>
+    <sheetView tabSelected="1" topLeftCell="A290" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="A304" sqref="A304:XFD304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2695,10 +2689,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="200" t="s">
+      <c r="A1" s="198" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="200" t="s">
+      <c r="B1" s="198" t="s">
         <v>654</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -5173,7 +5167,7 @@
       <c r="K75" s="4"/>
     </row>
     <row r="76" spans="1:11" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="12" t="s">
+      <c r="A76" s="11" t="s">
         <v>261</v>
       </c>
       <c r="B76" s="5" t="s">
@@ -5206,7 +5200,7 @@
       <c r="K76" s="4"/>
     </row>
     <row r="77" spans="1:11" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="12" t="s">
+      <c r="A77" s="11" t="s">
         <v>263</v>
       </c>
       <c r="B77" s="5" t="s">
@@ -5468,8 +5462,8 @@
         <v>83</v>
       </c>
       <c r="K84" s="4"/>
-      <c r="L84" s="9"/>
-      <c r="M84" s="9"/>
+      <c r="L84" s="8"/>
+      <c r="M84" s="8"/>
     </row>
     <row r="85" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
@@ -5502,9 +5496,9 @@
       <c r="J85" s="4">
         <v>84</v>
       </c>
-      <c r="K85" s="202"/>
-      <c r="L85" s="9"/>
-      <c r="M85" s="9"/>
+      <c r="K85" s="200"/>
+      <c r="L85" s="8"/>
+      <c r="M85" s="8"/>
     </row>
     <row r="86" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
@@ -5538,8 +5532,8 @@
         <v>85</v>
       </c>
       <c r="K86" s="4"/>
-      <c r="L86" s="9"/>
-      <c r="M86" s="9"/>
+      <c r="L86" s="8"/>
+      <c r="M86" s="8"/>
     </row>
     <row r="87" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
@@ -5573,8 +5567,8 @@
         <v>86</v>
       </c>
       <c r="K87" s="4"/>
-      <c r="L87" s="9"/>
-      <c r="M87" s="9"/>
+      <c r="L87" s="8"/>
+      <c r="M87" s="8"/>
     </row>
     <row r="88" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
@@ -5608,10 +5602,10 @@
         <v>87</v>
       </c>
       <c r="K88" s="4"/>
-      <c r="L88" s="9"/>
-      <c r="M88" s="9"/>
-    </row>
-    <row r="89" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L88" s="8"/>
+      <c r="M88" s="8"/>
+    </row>
+    <row r="89" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>282</v>
       </c>
@@ -5644,7 +5638,7 @@
       </c>
       <c r="K89" s="4"/>
     </row>
-    <row r="90" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>283</v>
       </c>
@@ -5677,7 +5671,7 @@
       </c>
       <c r="K90" s="4"/>
     </row>
-    <row r="91" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>284</v>
       </c>
@@ -5710,7 +5704,7 @@
       </c>
       <c r="K91" s="4"/>
     </row>
-    <row r="92" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>286</v>
       </c>
@@ -5743,47 +5737,47 @@
       </c>
       <c r="K92" s="4"/>
     </row>
-    <row r="93" spans="1:13" s="201" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="202" t="s">
+    <row r="93" spans="1:13" s="199" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="200" t="s">
         <v>385</v>
       </c>
-      <c r="B93" s="202" t="s">
+      <c r="B93" s="200" t="s">
         <v>384</v>
       </c>
-      <c r="C93" s="202" t="s">
+      <c r="C93" s="200" t="s">
         <v>23</v>
       </c>
-      <c r="D93" s="202">
+      <c r="D93" s="200">
         <v>2016</v>
       </c>
-      <c r="E93" s="202">
+      <c r="E93" s="200">
         <v>6</v>
       </c>
-      <c r="F93" s="202">
-        <v>1</v>
-      </c>
-      <c r="G93" s="202">
-        <v>0</v>
-      </c>
-      <c r="H93" s="202">
-        <v>1</v>
-      </c>
-      <c r="I93" s="202">
-        <v>0</v>
-      </c>
-      <c r="J93" s="202" t="s">
-        <v>135</v>
-      </c>
-      <c r="K93" s="202" t="s">
+      <c r="F93" s="200">
+        <v>1</v>
+      </c>
+      <c r="G93" s="200">
+        <v>0</v>
+      </c>
+      <c r="H93" s="200">
+        <v>1</v>
+      </c>
+      <c r="I93" s="200">
+        <v>0</v>
+      </c>
+      <c r="J93" s="200" t="s">
+        <v>135</v>
+      </c>
+      <c r="K93" s="200" t="s">
         <v>655</v>
       </c>
-      <c r="L93" s="202"/>
+      <c r="L93" s="200"/>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A94" s="15" t="s">
+      <c r="A94" s="14" t="s">
         <v>291</v>
       </c>
-      <c r="B94" s="15" t="s">
+      <c r="B94" s="14" t="s">
         <v>292</v>
       </c>
       <c r="C94" s="4" t="s">
@@ -5813,11 +5807,11 @@
       <c r="K94" s="4"/>
       <c r="L94" s="4"/>
     </row>
-    <row r="95" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="15" t="s">
+    <row r="95" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="14" t="s">
         <v>290</v>
       </c>
-      <c r="B95" s="15" t="s">
+      <c r="B95" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C95" s="4" t="s">
@@ -5848,10 +5842,10 @@
       <c r="L95" s="4"/>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A96" s="15" t="s">
+      <c r="A96" s="14" t="s">
         <v>293</v>
       </c>
-      <c r="B96" s="15" t="s">
+      <c r="B96" s="14" t="s">
         <v>294</v>
       </c>
       <c r="C96" s="4" t="s">
@@ -5987,7 +5981,7 @@
       <c r="A100" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="B100" s="14" t="s">
+      <c r="B100" s="13" t="s">
         <v>302</v>
       </c>
       <c r="C100" s="4" t="s">
@@ -6018,10 +6012,10 @@
       <c r="L100" s="4"/>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A101" s="22" t="s">
+      <c r="A101" s="20" t="s">
         <v>301</v>
       </c>
-      <c r="B101" s="13" t="s">
+      <c r="B101" s="12" t="s">
         <v>299</v>
       </c>
       <c r="C101" s="4" t="s">
@@ -6051,77 +6045,78 @@
       <c r="K101" s="4"/>
       <c r="L101" s="4"/>
     </row>
-    <row r="102" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="34" t="s">
+    <row r="102" spans="1:12" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="B102" s="34" t="s">
+      <c r="B102" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C102" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="D102" s="34">
+      <c r="C102" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D102" s="32">
         <v>2016</v>
       </c>
-      <c r="E102" s="34">
-        <v>3</v>
-      </c>
-      <c r="F102" s="34">
-        <v>0</v>
-      </c>
-      <c r="G102" s="34">
-        <v>0</v>
-      </c>
-      <c r="H102" s="34">
-        <v>0</v>
-      </c>
-      <c r="I102" s="34">
-        <v>0</v>
-      </c>
-      <c r="J102" s="34" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="22" t="s">
+      <c r="E102" s="32">
+        <v>3</v>
+      </c>
+      <c r="F102" s="32">
+        <v>0</v>
+      </c>
+      <c r="G102" s="32">
+        <v>0</v>
+      </c>
+      <c r="H102" s="32">
+        <v>0</v>
+      </c>
+      <c r="I102" s="32">
+        <v>0</v>
+      </c>
+      <c r="J102" s="32" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" s="200" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="200" t="s">
         <v>320</v>
       </c>
-      <c r="B103" s="18" t="s">
+      <c r="B103" s="200" t="s">
         <v>318</v>
       </c>
-      <c r="C103" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D103" s="4">
+      <c r="C103" s="200" t="s">
+        <v>3</v>
+      </c>
+      <c r="D103" s="200">
         <v>2016</v>
       </c>
-      <c r="E103" s="4">
+      <c r="E103" s="200">
         <v>4</v>
       </c>
-      <c r="F103" s="4">
-        <v>1</v>
-      </c>
-      <c r="G103" s="4">
-        <v>1</v>
-      </c>
-      <c r="H103" s="4">
-        <v>0</v>
-      </c>
-      <c r="I103" s="4">
-        <v>0</v>
-      </c>
-      <c r="J103" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="K103" s="4"/>
-      <c r="L103" s="4"/>
+      <c r="F103" s="200">
+        <v>1</v>
+      </c>
+      <c r="G103" s="200">
+        <v>0</v>
+      </c>
+      <c r="H103" s="200">
+        <v>0</v>
+      </c>
+      <c r="I103" s="200">
+        <v>0</v>
+      </c>
+      <c r="J103" s="200" t="s">
+        <v>135</v>
+      </c>
+      <c r="K103" s="198" t="s">
+        <v>656</v>
+      </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A104" s="22" t="s">
+      <c r="A104" s="20" t="s">
         <v>322</v>
       </c>
-      <c r="B104" s="19" t="s">
+      <c r="B104" s="17" t="s">
         <v>321</v>
       </c>
       <c r="C104" s="4" t="s">
@@ -6152,10 +6147,10 @@
       <c r="L104" s="4"/>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A105" s="22" t="s">
+      <c r="A105" s="20" t="s">
         <v>324</v>
       </c>
-      <c r="B105" s="21" t="s">
+      <c r="B105" s="19" t="s">
         <v>319</v>
       </c>
       <c r="C105" s="4" t="s">
@@ -6186,10 +6181,10 @@
       <c r="L105" s="4"/>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A106" s="22" t="s">
+      <c r="A106" s="20" t="s">
         <v>326</v>
       </c>
-      <c r="B106" s="22" t="s">
+      <c r="B106" s="20" t="s">
         <v>325</v>
       </c>
       <c r="C106" s="4" t="s">
@@ -6220,10 +6215,10 @@
       <c r="L106" s="4"/>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A107" s="22" t="s">
+      <c r="A107" s="20" t="s">
         <v>317</v>
       </c>
-      <c r="B107" s="19" t="s">
+      <c r="B107" s="17" t="s">
         <v>316</v>
       </c>
       <c r="C107" s="4" t="s">
@@ -6254,10 +6249,10 @@
       <c r="L107" s="4"/>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A108" s="22" t="s">
+      <c r="A108" s="20" t="s">
         <v>315</v>
       </c>
-      <c r="B108" s="17" t="s">
+      <c r="B108" s="16" t="s">
         <v>306</v>
       </c>
       <c r="C108" s="4" t="s">
@@ -6287,11 +6282,11 @@
       <c r="K108" s="4"/>
       <c r="L108" s="4"/>
     </row>
-    <row r="109" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="22" t="s">
+    <row r="109" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="B109" s="16" t="s">
+      <c r="B109" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C109" s="4" t="s">
@@ -6322,10 +6317,10 @@
       <c r="L109" s="4"/>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A110" s="22" t="s">
+      <c r="A110" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="B110" s="20" t="s">
+      <c r="B110" s="18" t="s">
         <v>16</v>
       </c>
       <c r="C110" s="4" t="s">
@@ -6356,10 +6351,10 @@
       <c r="L110" s="4"/>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A111" s="29" t="s">
+      <c r="A111" s="27" t="s">
         <v>335</v>
       </c>
-      <c r="B111" s="29" t="s">
+      <c r="B111" s="27" t="s">
         <v>307</v>
       </c>
       <c r="C111" s="4" t="s">
@@ -6393,7 +6388,7 @@
       <c r="A112" s="5" t="s">
         <v>331</v>
       </c>
-      <c r="B112" s="26" t="s">
+      <c r="B112" s="24" t="s">
         <v>17</v>
       </c>
       <c r="C112" s="4" t="s">
@@ -6427,7 +6422,7 @@
       <c r="A113" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="B113" s="25" t="s">
+      <c r="B113" s="23" t="s">
         <v>18</v>
       </c>
       <c r="C113" s="4" t="s">
@@ -6457,11 +6452,11 @@
       <c r="K113" s="4"/>
       <c r="L113" s="4"/>
     </row>
-    <row r="114" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="28" t="s">
+    <row r="114" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="26" t="s">
         <v>333</v>
       </c>
-      <c r="B114" s="28" t="s">
+      <c r="B114" s="26" t="s">
         <v>308</v>
       </c>
       <c r="C114" s="4" t="s">
@@ -6491,35 +6486,35 @@
       <c r="K114" s="4"/>
       <c r="L114" s="4"/>
     </row>
-    <row r="115" spans="1:12" s="203" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="203" t="s">
+    <row r="115" spans="1:12" s="201" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="201" t="s">
         <v>334</v>
       </c>
-      <c r="B115" s="203" t="s">
+      <c r="B115" s="201" t="s">
         <v>309</v>
       </c>
-      <c r="C115" s="203" t="s">
-        <v>3</v>
-      </c>
-      <c r="D115" s="203">
+      <c r="C115" s="201" t="s">
+        <v>3</v>
+      </c>
+      <c r="D115" s="201">
         <v>2016</v>
       </c>
-      <c r="E115" s="203">
+      <c r="E115" s="201">
         <v>5</v>
       </c>
-      <c r="F115" s="203">
-        <v>0</v>
-      </c>
-      <c r="G115" s="203">
-        <v>0</v>
-      </c>
-      <c r="H115" s="203">
-        <v>0</v>
-      </c>
-      <c r="I115" s="203">
-        <v>0</v>
-      </c>
-      <c r="J115" s="203" t="s">
+      <c r="F115" s="201">
+        <v>0</v>
+      </c>
+      <c r="G115" s="201">
+        <v>0</v>
+      </c>
+      <c r="H115" s="201">
+        <v>0</v>
+      </c>
+      <c r="I115" s="201">
+        <v>0</v>
+      </c>
+      <c r="J115" s="201" t="s">
         <v>135</v>
       </c>
     </row>
@@ -6527,7 +6522,7 @@
       <c r="A116" s="5" t="s">
         <v>329</v>
       </c>
-      <c r="B116" s="24" t="s">
+      <c r="B116" s="22" t="s">
         <v>328</v>
       </c>
       <c r="C116" s="4" t="s">
@@ -6561,7 +6556,7 @@
       <c r="A117" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="B117" s="23" t="s">
+      <c r="B117" s="21" t="s">
         <v>310</v>
       </c>
       <c r="C117" s="4" t="s">
@@ -6595,7 +6590,7 @@
       <c r="A118" s="5" t="s">
         <v>332</v>
       </c>
-      <c r="B118" s="27" t="s">
+      <c r="B118" s="25" t="s">
         <v>19</v>
       </c>
       <c r="C118" s="4" t="s">
@@ -6629,7 +6624,7 @@
       <c r="A119" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="B119" s="30" t="s">
+      <c r="B119" s="28" t="s">
         <v>311</v>
       </c>
       <c r="C119" s="4" t="s">
@@ -6660,10 +6655,10 @@
       <c r="L119" s="4"/>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A120" s="34" t="s">
+      <c r="A120" s="32" t="s">
         <v>337</v>
       </c>
-      <c r="B120" s="34" t="s">
+      <c r="B120" s="32" t="s">
         <v>20</v>
       </c>
       <c r="C120" s="4" t="s">
@@ -6695,10 +6690,10 @@
       <c r="L120" s="4"/>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A121" s="34" t="s">
+      <c r="A121" s="32" t="s">
         <v>339</v>
       </c>
-      <c r="B121" s="34" t="s">
+      <c r="B121" s="32" t="s">
         <v>338</v>
       </c>
       <c r="C121" s="4" t="s">
@@ -6728,11 +6723,11 @@
       <c r="K121" s="4"/>
       <c r="L121" s="4"/>
     </row>
-    <row r="122" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="34" t="s">
+    <row r="122" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="32" t="s">
         <v>341</v>
       </c>
-      <c r="B122" s="34" t="s">
+      <c r="B122" s="32" t="s">
         <v>312</v>
       </c>
       <c r="C122" s="4" t="s">
@@ -6763,10 +6758,10 @@
       <c r="L122" s="4"/>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A123" s="34" t="s">
+      <c r="A123" s="32" t="s">
         <v>343</v>
       </c>
-      <c r="B123" s="34" t="s">
+      <c r="B123" s="32" t="s">
         <v>24</v>
       </c>
       <c r="C123" s="4" t="s">
@@ -6798,10 +6793,10 @@
       <c r="L123" s="4"/>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A124" s="34" t="s">
+      <c r="A124" s="32" t="s">
         <v>342</v>
       </c>
-      <c r="B124" s="34" t="s">
+      <c r="B124" s="32" t="s">
         <v>313</v>
       </c>
       <c r="C124" s="4" t="s">
@@ -6832,10 +6827,10 @@
       <c r="L124" s="4"/>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A125" s="34" t="s">
+      <c r="A125" s="32" t="s">
         <v>340</v>
       </c>
-      <c r="B125" s="34" t="s">
+      <c r="B125" s="32" t="s">
         <v>314</v>
       </c>
       <c r="C125" s="4" t="s">
@@ -6867,10 +6862,10 @@
       <c r="L125" s="4"/>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A126" s="34" t="s">
+      <c r="A126" s="32" t="s">
         <v>345</v>
       </c>
-      <c r="B126" s="34" t="s">
+      <c r="B126" s="32" t="s">
         <v>344</v>
       </c>
       <c r="C126" s="4" t="s">
@@ -6902,10 +6897,10 @@
       <c r="L126" s="4"/>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A127" s="34" t="s">
+      <c r="A127" s="32" t="s">
         <v>356</v>
       </c>
-      <c r="B127" s="34" t="s">
+      <c r="B127" s="32" t="s">
         <v>25</v>
       </c>
       <c r="C127" s="4" t="s">
@@ -6936,10 +6931,10 @@
       <c r="L127" s="4"/>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A128" s="34" t="s">
+      <c r="A128" s="32" t="s">
         <v>354</v>
       </c>
-      <c r="B128" s="34" t="s">
+      <c r="B128" s="32" t="s">
         <v>352</v>
       </c>
       <c r="C128" s="4" t="s">
@@ -6970,10 +6965,10 @@
       <c r="L128" s="4"/>
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A129" s="34" t="s">
+      <c r="A129" s="32" t="s">
         <v>350</v>
       </c>
-      <c r="B129" s="34" t="s">
+      <c r="B129" s="32" t="s">
         <v>26</v>
       </c>
       <c r="C129" s="4" t="s">
@@ -7005,10 +7000,10 @@
       <c r="L129" s="4"/>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A130" s="34" t="s">
+      <c r="A130" s="32" t="s">
         <v>351</v>
       </c>
-      <c r="B130" s="34" t="s">
+      <c r="B130" s="32" t="s">
         <v>27</v>
       </c>
       <c r="C130" s="4" t="s">
@@ -7039,10 +7034,10 @@
       <c r="L130" s="4"/>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A131" s="34" t="s">
+      <c r="A131" s="32" t="s">
         <v>355</v>
       </c>
-      <c r="B131" s="34" t="s">
+      <c r="B131" s="32" t="s">
         <v>353</v>
       </c>
       <c r="C131" s="4" t="s">
@@ -7073,10 +7068,10 @@
       <c r="L131" s="4"/>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A132" s="34" t="s">
+      <c r="A132" s="32" t="s">
         <v>349</v>
       </c>
-      <c r="B132" s="34" t="s">
+      <c r="B132" s="32" t="s">
         <v>346</v>
       </c>
       <c r="C132" s="4" t="s">
@@ -7107,10 +7102,10 @@
       <c r="L132" s="4"/>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A133" s="34" t="s">
+      <c r="A133" s="32" t="s">
         <v>361</v>
       </c>
-      <c r="B133" s="34" t="s">
+      <c r="B133" s="32" t="s">
         <v>347</v>
       </c>
       <c r="C133" s="4" t="s">
@@ -7140,11 +7135,11 @@
       <c r="K133" s="4"/>
       <c r="L133" s="4"/>
     </row>
-    <row r="134" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="34" t="s">
+    <row r="134" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="32" t="s">
         <v>360</v>
       </c>
-      <c r="B134" s="34" t="s">
+      <c r="B134" s="32" t="s">
         <v>359</v>
       </c>
       <c r="C134" s="4" t="s">
@@ -7175,10 +7170,10 @@
       <c r="L134" s="4"/>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A135" s="34" t="s">
+      <c r="A135" s="32" t="s">
         <v>358</v>
       </c>
-      <c r="B135" s="34" t="s">
+      <c r="B135" s="32" t="s">
         <v>357</v>
       </c>
       <c r="C135" s="4" t="s">
@@ -7209,10 +7204,10 @@
       <c r="L135" s="4"/>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A136" s="34" t="s">
+      <c r="A136" s="32" t="s">
         <v>365</v>
       </c>
-      <c r="B136" s="34" t="s">
+      <c r="B136" s="32" t="s">
         <v>364</v>
       </c>
       <c r="C136" s="4" t="s">
@@ -7246,7 +7241,7 @@
       <c r="A137" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="B137" s="33" t="s">
+      <c r="B137" s="31" t="s">
         <v>366</v>
       </c>
       <c r="C137" s="4" t="s">
@@ -7280,7 +7275,7 @@
       <c r="A138" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="B138" s="35" t="s">
+      <c r="B138" s="33" t="s">
         <v>29</v>
       </c>
       <c r="C138" s="4" t="s">
@@ -7314,7 +7309,7 @@
       <c r="A139" s="5" t="s">
         <v>363</v>
       </c>
-      <c r="B139" s="32" t="s">
+      <c r="B139" s="30" t="s">
         <v>348</v>
       </c>
       <c r="C139" s="4" t="s">
@@ -7348,7 +7343,7 @@
       <c r="A140" s="5" t="s">
         <v>362</v>
       </c>
-      <c r="B140" s="31" t="s">
+      <c r="B140" s="29" t="s">
         <v>30</v>
       </c>
       <c r="C140" s="4" t="s">
@@ -7382,7 +7377,7 @@
       <c r="A141" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="B141" s="38" t="s">
+      <c r="B141" s="36" t="s">
         <v>373</v>
       </c>
       <c r="C141" s="4" t="s">
@@ -7416,7 +7411,7 @@
       <c r="A142" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="B142" s="40" t="s">
+      <c r="B142" s="38" t="s">
         <v>376</v>
       </c>
       <c r="C142" s="4" t="s">
@@ -7450,7 +7445,7 @@
       <c r="A143" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="B143" s="36" t="s">
+      <c r="B143" s="34" t="s">
         <v>369</v>
       </c>
       <c r="C143" s="4" t="s">
@@ -7484,7 +7479,7 @@
       <c r="A144" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="B144" s="39" t="s">
+      <c r="B144" s="37" t="s">
         <v>370</v>
       </c>
       <c r="C144" s="4" t="s">
@@ -7518,7 +7513,7 @@
       <c r="A145" s="5" t="s">
         <v>372</v>
       </c>
-      <c r="B145" s="37" t="s">
+      <c r="B145" s="35" t="s">
         <v>31</v>
       </c>
       <c r="C145" s="4" t="s">
@@ -7552,7 +7547,7 @@
       <c r="A146" s="5" t="s">
         <v>383</v>
       </c>
-      <c r="B146" s="41" t="s">
+      <c r="B146" s="39" t="s">
         <v>380</v>
       </c>
       <c r="C146" s="4" t="s">
@@ -7583,10 +7578,10 @@
       <c r="L146" s="4"/>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A147" s="41" t="s">
+      <c r="A147" s="39" t="s">
         <v>379</v>
       </c>
-      <c r="B147" s="41" t="s">
+      <c r="B147" s="39" t="s">
         <v>378</v>
       </c>
       <c r="C147" s="4" t="s">
@@ -7617,10 +7612,10 @@
       <c r="L147" s="4"/>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A148" s="44" t="s">
+      <c r="A148" s="42" t="s">
         <v>388</v>
       </c>
-      <c r="B148" s="43" t="s">
+      <c r="B148" s="41" t="s">
         <v>35</v>
       </c>
       <c r="C148" s="4" t="s">
@@ -7651,10 +7646,10 @@
       <c r="L148" s="4"/>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A149" s="44" t="s">
+      <c r="A149" s="42" t="s">
         <v>386</v>
       </c>
-      <c r="B149" s="42" t="s">
+      <c r="B149" s="40" t="s">
         <v>37</v>
       </c>
       <c r="C149" s="4" t="s">
@@ -7685,10 +7680,10 @@
       <c r="L149" s="4"/>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A150" s="46" t="s">
+      <c r="A150" s="44" t="s">
         <v>390</v>
       </c>
-      <c r="B150" s="44" t="s">
+      <c r="B150" s="42" t="s">
         <v>381</v>
       </c>
       <c r="C150" s="4" t="s">
@@ -7719,10 +7714,10 @@
       <c r="L150" s="4"/>
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A151" s="46" t="s">
+      <c r="A151" s="44" t="s">
         <v>389</v>
       </c>
-      <c r="B151" s="44" t="s">
+      <c r="B151" s="42" t="s">
         <v>38</v>
       </c>
       <c r="C151" s="4" t="s">
@@ -7753,7 +7748,7 @@
       <c r="L151" s="4"/>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A152" s="46" t="s">
+      <c r="A152" s="44" t="s">
         <v>401</v>
       </c>
       <c r="B152" s="5" t="s">
@@ -7787,10 +7782,10 @@
       <c r="L152" s="4"/>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A153" s="46" t="s">
+      <c r="A153" s="44" t="s">
         <v>387</v>
       </c>
-      <c r="B153" s="44" t="s">
+      <c r="B153" s="42" t="s">
         <v>40</v>
       </c>
       <c r="C153" s="4" t="s">
@@ -7821,10 +7816,10 @@
       <c r="L153" s="4"/>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A154" s="46" t="s">
+      <c r="A154" s="44" t="s">
         <v>392</v>
       </c>
-      <c r="B154" s="45" t="s">
+      <c r="B154" s="43" t="s">
         <v>382</v>
       </c>
       <c r="C154" s="4" t="s">
@@ -7854,11 +7849,11 @@
       <c r="K154" s="4"/>
       <c r="L154" s="4"/>
     </row>
-    <row r="155" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A155" s="46" t="s">
+    <row r="155" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="44" t="s">
         <v>391</v>
       </c>
-      <c r="B155" s="45" t="s">
+      <c r="B155" s="43" t="s">
         <v>42</v>
       </c>
       <c r="C155" s="4" t="s">
@@ -7889,10 +7884,10 @@
       <c r="L155" s="4"/>
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A156" s="46" t="s">
+      <c r="A156" s="44" t="s">
         <v>397</v>
       </c>
-      <c r="B156" s="46" t="s">
+      <c r="B156" s="44" t="s">
         <v>44</v>
       </c>
       <c r="C156" s="4" t="s">
@@ -7957,10 +7952,10 @@
       <c r="L157" s="4"/>
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A158" s="44" t="s">
+      <c r="A158" s="42" t="s">
         <v>396</v>
       </c>
-      <c r="B158" s="46" t="s">
+      <c r="B158" s="44" t="s">
         <v>46</v>
       </c>
       <c r="C158" s="4" t="s">
@@ -7991,10 +7986,10 @@
       <c r="L158" s="4"/>
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A159" s="53" t="s">
+      <c r="A159" s="51" t="s">
         <v>394</v>
       </c>
-      <c r="B159" s="46" t="s">
+      <c r="B159" s="44" t="s">
         <v>393</v>
       </c>
       <c r="C159" s="4" t="s">
@@ -8025,10 +8020,10 @@
       <c r="L159" s="4"/>
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A160" s="53" t="s">
+      <c r="A160" s="51" t="s">
         <v>399</v>
       </c>
-      <c r="B160" s="46" t="s">
+      <c r="B160" s="44" t="s">
         <v>398</v>
       </c>
       <c r="C160" s="4" t="s">
@@ -8059,10 +8054,10 @@
       <c r="L160" s="4"/>
     </row>
     <row r="161" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A161" s="53" t="s">
+      <c r="A161" s="51" t="s">
         <v>400</v>
       </c>
-      <c r="B161" s="46" t="s">
+      <c r="B161" s="44" t="s">
         <v>47</v>
       </c>
       <c r="C161" s="4" t="s">
@@ -8093,10 +8088,10 @@
       <c r="L161" s="4"/>
     </row>
     <row r="162" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A162" s="53" t="s">
+      <c r="A162" s="51" t="s">
         <v>408</v>
       </c>
-      <c r="B162" s="48" t="s">
+      <c r="B162" s="46" t="s">
         <v>403</v>
       </c>
       <c r="C162" s="4" t="s">
@@ -8127,10 +8122,10 @@
       <c r="L162" s="4"/>
     </row>
     <row r="163" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A163" s="53" t="s">
+      <c r="A163" s="51" t="s">
         <v>402</v>
       </c>
-      <c r="B163" s="47" t="s">
+      <c r="B163" s="45" t="s">
         <v>48</v>
       </c>
       <c r="C163" s="4" t="s">
@@ -8160,11 +8155,11 @@
       <c r="K163" s="4"/>
       <c r="L163" s="4"/>
     </row>
-    <row r="164" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="53" t="s">
+    <row r="164" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="51" t="s">
         <v>412</v>
       </c>
-      <c r="B164" s="51" t="s">
+      <c r="B164" s="49" t="s">
         <v>49</v>
       </c>
       <c r="C164" s="4" t="s">
@@ -8195,10 +8190,10 @@
       <c r="L164" s="4"/>
     </row>
     <row r="165" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A165" s="53" t="s">
+      <c r="A165" s="51" t="s">
         <v>411</v>
       </c>
-      <c r="B165" s="50" t="s">
+      <c r="B165" s="48" t="s">
         <v>410</v>
       </c>
       <c r="C165" s="4" t="s">
@@ -8232,7 +8227,7 @@
       <c r="A166" s="5" t="s">
         <v>409</v>
       </c>
-      <c r="B166" s="49" t="s">
+      <c r="B166" s="47" t="s">
         <v>50</v>
       </c>
       <c r="C166" s="4" t="s">
@@ -8266,7 +8261,7 @@
       <c r="A167" s="5" t="s">
         <v>413</v>
       </c>
-      <c r="B167" s="52" t="s">
+      <c r="B167" s="50" t="s">
         <v>51</v>
       </c>
       <c r="C167" s="4" t="s">
@@ -8300,7 +8295,7 @@
       <c r="A168" s="5" t="s">
         <v>414</v>
       </c>
-      <c r="B168" s="53" t="s">
+      <c r="B168" s="51" t="s">
         <v>404</v>
       </c>
       <c r="C168" s="4" t="s">
@@ -8334,7 +8329,7 @@
       <c r="A169" s="5" t="s">
         <v>418</v>
       </c>
-      <c r="B169" s="57" t="s">
+      <c r="B169" s="55" t="s">
         <v>52</v>
       </c>
       <c r="C169" s="4" t="s">
@@ -8368,7 +8363,7 @@
       <c r="A170" s="5" t="s">
         <v>416</v>
       </c>
-      <c r="B170" s="55" t="s">
+      <c r="B170" s="53" t="s">
         <v>53</v>
       </c>
       <c r="C170" s="4" t="s">
@@ -8402,7 +8397,7 @@
       <c r="A171" s="5" t="s">
         <v>415</v>
       </c>
-      <c r="B171" s="54" t="s">
+      <c r="B171" s="52" t="s">
         <v>405</v>
       </c>
       <c r="C171" s="4" t="s">
@@ -8436,7 +8431,7 @@
       <c r="A172" s="5" t="s">
         <v>417</v>
       </c>
-      <c r="B172" s="56" t="s">
+      <c r="B172" s="54" t="s">
         <v>54</v>
       </c>
       <c r="C172" s="4" t="s">
@@ -8470,7 +8465,7 @@
       <c r="A173" s="5" t="s">
         <v>421</v>
       </c>
-      <c r="B173" s="58" t="s">
+      <c r="B173" s="56" t="s">
         <v>422</v>
       </c>
       <c r="C173" s="4" t="s">
@@ -8504,7 +8499,7 @@
       <c r="A174" s="5" t="s">
         <v>424</v>
       </c>
-      <c r="B174" s="59" t="s">
+      <c r="B174" s="57" t="s">
         <v>423</v>
       </c>
       <c r="C174" s="4" t="s">
@@ -8572,7 +8567,7 @@
       <c r="A176" s="5" t="s">
         <v>425</v>
       </c>
-      <c r="B176" s="60" t="s">
+      <c r="B176" s="58" t="s">
         <v>406</v>
       </c>
       <c r="C176" s="4" t="s">
@@ -8606,7 +8601,7 @@
       <c r="A177" s="5" t="s">
         <v>426</v>
       </c>
-      <c r="B177" s="61" t="s">
+      <c r="B177" s="59" t="s">
         <v>407</v>
       </c>
       <c r="C177" s="4" t="s">
@@ -8640,7 +8635,7 @@
       <c r="A178" s="5" t="s">
         <v>427</v>
       </c>
-      <c r="B178" s="62" t="s">
+      <c r="B178" s="60" t="s">
         <v>57</v>
       </c>
       <c r="C178" s="4" t="s">
@@ -8674,7 +8669,7 @@
       <c r="A179" s="5" t="s">
         <v>436</v>
       </c>
-      <c r="B179" s="68" t="s">
+      <c r="B179" s="66" t="s">
         <v>58</v>
       </c>
       <c r="C179" s="4" t="s">
@@ -8708,7 +8703,7 @@
       <c r="A180" s="5" t="s">
         <v>434</v>
       </c>
-      <c r="B180" s="66" t="s">
+      <c r="B180" s="64" t="s">
         <v>433</v>
       </c>
       <c r="C180" s="4" t="s">
@@ -8742,13 +8737,13 @@
       <c r="A181" s="5" t="s">
         <v>430</v>
       </c>
-      <c r="B181" s="64" t="s">
+      <c r="B181" s="62" t="s">
         <v>429</v>
       </c>
       <c r="C181" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D181" s="72">
+      <c r="D181" s="70">
         <v>2015</v>
       </c>
       <c r="E181" s="4">
@@ -8776,7 +8771,7 @@
       <c r="A182" s="5" t="s">
         <v>432</v>
       </c>
-      <c r="B182" s="65" t="s">
+      <c r="B182" s="63" t="s">
         <v>431</v>
       </c>
       <c r="C182" s="4" t="s">
@@ -8810,7 +8805,7 @@
       <c r="A183" s="5" t="s">
         <v>435</v>
       </c>
-      <c r="B183" s="67" t="s">
+      <c r="B183" s="65" t="s">
         <v>60</v>
       </c>
       <c r="C183" s="4" t="s">
@@ -8844,7 +8839,7 @@
       <c r="A184" s="5" t="s">
         <v>428</v>
       </c>
-      <c r="B184" s="63" t="s">
+      <c r="B184" s="61" t="s">
         <v>61</v>
       </c>
       <c r="C184" s="4" t="s">
@@ -8878,7 +8873,7 @@
       <c r="A185" s="5" t="s">
         <v>445</v>
       </c>
-      <c r="B185" s="71" t="s">
+      <c r="B185" s="69" t="s">
         <v>62</v>
       </c>
       <c r="C185" s="4" t="s">
@@ -8912,7 +8907,7 @@
       <c r="A186" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="B186" s="72" t="s">
+      <c r="B186" s="70" t="s">
         <v>448</v>
       </c>
       <c r="C186" s="4" t="s">
@@ -8946,7 +8941,7 @@
       <c r="A187" s="5" t="s">
         <v>447</v>
       </c>
-      <c r="B187" s="72" t="s">
+      <c r="B187" s="70" t="s">
         <v>446</v>
       </c>
       <c r="C187" s="4" t="s">
@@ -8980,7 +8975,7 @@
       <c r="A188" s="5" t="s">
         <v>450</v>
       </c>
-      <c r="B188" s="69" t="s">
+      <c r="B188" s="67" t="s">
         <v>63</v>
       </c>
       <c r="C188" s="4" t="s">
@@ -9014,7 +9009,7 @@
       <c r="A189" s="5" t="s">
         <v>444</v>
       </c>
-      <c r="B189" s="70" t="s">
+      <c r="B189" s="68" t="s">
         <v>437</v>
       </c>
       <c r="C189" s="4" t="s">
@@ -9048,7 +9043,7 @@
       <c r="A190" s="5" t="s">
         <v>457</v>
       </c>
-      <c r="B190" s="76" t="s">
+      <c r="B190" s="74" t="s">
         <v>64</v>
       </c>
       <c r="C190" s="4" t="s">
@@ -9082,7 +9077,7 @@
       <c r="A191" s="5" t="s">
         <v>453</v>
       </c>
-      <c r="B191" s="74" t="s">
+      <c r="B191" s="72" t="s">
         <v>438</v>
       </c>
       <c r="C191" s="4" t="s">
@@ -9116,7 +9111,7 @@
       <c r="A192" s="5" t="s">
         <v>454</v>
       </c>
-      <c r="B192" s="75" t="s">
+      <c r="B192" s="73" t="s">
         <v>65</v>
       </c>
       <c r="C192" s="4" t="s">
@@ -9150,7 +9145,7 @@
       <c r="A193" s="5" t="s">
         <v>451</v>
       </c>
-      <c r="B193" s="73" t="s">
+      <c r="B193" s="71" t="s">
         <v>66</v>
       </c>
       <c r="C193" s="4" t="s">
@@ -9184,7 +9179,7 @@
       <c r="A194" s="5" t="s">
         <v>456</v>
       </c>
-      <c r="B194" s="75" t="s">
+      <c r="B194" s="73" t="s">
         <v>455</v>
       </c>
       <c r="C194" s="4" t="s">
@@ -9218,7 +9213,7 @@
       <c r="A195" s="5" t="s">
         <v>459</v>
       </c>
-      <c r="B195" s="78" t="s">
+      <c r="B195" s="76" t="s">
         <v>439</v>
       </c>
       <c r="C195" s="4" t="s">
@@ -9252,7 +9247,7 @@
       <c r="A196" s="5" t="s">
         <v>461</v>
       </c>
-      <c r="B196" s="79" t="s">
+      <c r="B196" s="77" t="s">
         <v>67</v>
       </c>
       <c r="C196" s="4" t="s">
@@ -9286,7 +9281,7 @@
       <c r="A197" s="5" t="s">
         <v>463</v>
       </c>
-      <c r="B197" s="81" t="s">
+      <c r="B197" s="79" t="s">
         <v>462</v>
       </c>
       <c r="C197" s="4" t="s">
@@ -9320,7 +9315,7 @@
       <c r="A198" s="5" t="s">
         <v>464</v>
       </c>
-      <c r="B198" s="82" t="s">
+      <c r="B198" s="80" t="s">
         <v>68</v>
       </c>
       <c r="C198" s="4" t="s">
@@ -9354,7 +9349,7 @@
       <c r="A199" s="5" t="s">
         <v>466</v>
       </c>
-      <c r="B199" s="83" t="s">
+      <c r="B199" s="81" t="s">
         <v>465</v>
       </c>
       <c r="C199" s="4" t="s">
@@ -9388,7 +9383,7 @@
       <c r="A200" s="5" t="s">
         <v>458</v>
       </c>
-      <c r="B200" s="77" t="s">
+      <c r="B200" s="75" t="s">
         <v>69</v>
       </c>
       <c r="C200" s="4" t="s">
@@ -9422,7 +9417,7 @@
       <c r="A201" s="5" t="s">
         <v>460</v>
       </c>
-      <c r="B201" s="80" t="s">
+      <c r="B201" s="78" t="s">
         <v>440</v>
       </c>
       <c r="C201" s="4" t="s">
@@ -9456,7 +9451,7 @@
       <c r="A202" s="5" t="s">
         <v>467</v>
       </c>
-      <c r="B202" s="85" t="s">
+      <c r="B202" s="83" t="s">
         <v>441</v>
       </c>
       <c r="C202" s="4" t="s">
@@ -9490,7 +9485,7 @@
       <c r="A203" s="5" t="s">
         <v>470</v>
       </c>
-      <c r="B203" s="87" t="s">
+      <c r="B203" s="85" t="s">
         <v>70</v>
       </c>
       <c r="C203" s="4" t="s">
@@ -9524,7 +9519,7 @@
       <c r="A204" s="5" t="s">
         <v>468</v>
       </c>
-      <c r="B204" s="84" t="s">
+      <c r="B204" s="82" t="s">
         <v>71</v>
       </c>
       <c r="C204" s="4" t="s">
@@ -9558,7 +9553,7 @@
       <c r="A205" s="5" t="s">
         <v>469</v>
       </c>
-      <c r="B205" s="86" t="s">
+      <c r="B205" s="84" t="s">
         <v>72</v>
       </c>
       <c r="C205" s="4" t="s">
@@ -9592,7 +9587,7 @@
       <c r="A206" s="5" t="s">
         <v>471</v>
       </c>
-      <c r="B206" s="89" t="s">
+      <c r="B206" s="87" t="s">
         <v>74</v>
       </c>
       <c r="C206" s="4" t="s">
@@ -9626,7 +9621,7 @@
       <c r="A207" s="5" t="s">
         <v>475</v>
       </c>
-      <c r="B207" s="91" t="s">
+      <c r="B207" s="89" t="s">
         <v>442</v>
       </c>
       <c r="C207" s="4" t="s">
@@ -9660,7 +9655,7 @@
       <c r="A208" s="5" t="s">
         <v>473</v>
       </c>
-      <c r="B208" s="88" t="s">
+      <c r="B208" s="86" t="s">
         <v>75</v>
       </c>
       <c r="C208" s="4" t="s">
@@ -9694,7 +9689,7 @@
       <c r="A209" s="5" t="s">
         <v>472</v>
       </c>
-      <c r="B209" s="89" t="s">
+      <c r="B209" s="87" t="s">
         <v>76</v>
       </c>
       <c r="C209" s="4" t="s">
@@ -9728,7 +9723,7 @@
       <c r="A210" s="5" t="s">
         <v>474</v>
       </c>
-      <c r="B210" s="90" t="s">
+      <c r="B210" s="88" t="s">
         <v>77</v>
       </c>
       <c r="C210" s="4" t="s">
@@ -9762,7 +9757,7 @@
       <c r="A211" s="5" t="s">
         <v>476</v>
       </c>
-      <c r="B211" s="92" t="s">
+      <c r="B211" s="90" t="s">
         <v>443</v>
       </c>
       <c r="C211" s="4" t="s">
@@ -9796,7 +9791,7 @@
       <c r="A212" s="5" t="s">
         <v>483</v>
       </c>
-      <c r="B212" s="97" t="s">
+      <c r="B212" s="95" t="s">
         <v>78</v>
       </c>
       <c r="C212" s="4" t="s">
@@ -9830,7 +9825,7 @@
       <c r="A213" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="B213" s="96" t="s">
+      <c r="B213" s="94" t="s">
         <v>452</v>
       </c>
       <c r="C213" s="4" t="s">
@@ -9864,7 +9859,7 @@
       <c r="A214" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="B214" s="94" t="s">
+      <c r="B214" s="92" t="s">
         <v>479</v>
       </c>
       <c r="C214" s="4" t="s">
@@ -9898,7 +9893,7 @@
       <c r="A215" s="5" t="s">
         <v>477</v>
       </c>
-      <c r="B215" s="93" t="s">
+      <c r="B215" s="91" t="s">
         <v>478</v>
       </c>
       <c r="C215" s="4" t="s">
@@ -9932,7 +9927,7 @@
       <c r="A216" s="5" t="s">
         <v>482</v>
       </c>
-      <c r="B216" s="95" t="s">
+      <c r="B216" s="93" t="s">
         <v>79</v>
       </c>
       <c r="C216" s="4" t="s">
@@ -9966,7 +9961,7 @@
       <c r="A217" s="5" t="s">
         <v>493</v>
       </c>
-      <c r="B217" s="98" t="s">
+      <c r="B217" s="96" t="s">
         <v>492</v>
       </c>
       <c r="C217" s="4" t="s">
@@ -9997,10 +9992,10 @@
       <c r="L217" s="4"/>
     </row>
     <row r="218" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A218" s="101" t="s">
+      <c r="A218" s="99" t="s">
         <v>491</v>
       </c>
-      <c r="B218" s="101" t="s">
+      <c r="B218" s="99" t="s">
         <v>484</v>
       </c>
       <c r="C218" s="4" t="s">
@@ -10030,11 +10025,11 @@
       <c r="K218" s="4"/>
       <c r="L218" s="4"/>
     </row>
-    <row r="219" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A219" s="101" t="s">
+    <row r="219" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A219" s="99" t="s">
         <v>494</v>
       </c>
-      <c r="B219" s="101" t="s">
+      <c r="B219" s="99" t="s">
         <v>495</v>
       </c>
       <c r="C219" s="4" t="s">
@@ -10065,10 +10060,10 @@
       <c r="L219" s="4"/>
     </row>
     <row r="220" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A220" s="101" t="s">
+      <c r="A220" s="99" t="s">
         <v>501</v>
       </c>
-      <c r="B220" s="101" t="s">
+      <c r="B220" s="99" t="s">
         <v>500</v>
       </c>
       <c r="C220" s="4" t="s">
@@ -10099,10 +10094,10 @@
       <c r="L220" s="4"/>
     </row>
     <row r="221" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A221" s="101" t="s">
+      <c r="A221" s="99" t="s">
         <v>499</v>
       </c>
-      <c r="B221" s="101" t="s">
+      <c r="B221" s="99" t="s">
         <v>80</v>
       </c>
       <c r="C221" s="4" t="s">
@@ -10133,10 +10128,10 @@
       <c r="L221" s="4"/>
     </row>
     <row r="222" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A222" s="101" t="s">
+      <c r="A222" s="99" t="s">
         <v>502</v>
       </c>
-      <c r="B222" s="101" t="s">
+      <c r="B222" s="99" t="s">
         <v>485</v>
       </c>
       <c r="C222" s="4" t="s">
@@ -10167,10 +10162,10 @@
       <c r="L222" s="4"/>
     </row>
     <row r="223" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A223" s="101" t="s">
+      <c r="A223" s="99" t="s">
         <v>497</v>
       </c>
-      <c r="B223" s="101" t="s">
+      <c r="B223" s="99" t="s">
         <v>496</v>
       </c>
       <c r="C223" s="4" t="s">
@@ -10201,10 +10196,10 @@
       <c r="L223" s="4"/>
     </row>
     <row r="224" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A224" s="101" t="s">
+      <c r="A224" s="99" t="s">
         <v>498</v>
       </c>
-      <c r="B224" s="101" t="s">
+      <c r="B224" s="99" t="s">
         <v>82</v>
       </c>
       <c r="C224" s="4" t="s">
@@ -10234,11 +10229,11 @@
       <c r="K224" s="4"/>
       <c r="L224" s="4"/>
     </row>
-    <row r="225" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A225" s="101" t="s">
+    <row r="225" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A225" s="99" t="s">
         <v>506</v>
       </c>
-      <c r="B225" s="101" t="s">
+      <c r="B225" s="99" t="s">
         <v>505</v>
       </c>
       <c r="C225" s="4" t="s">
@@ -10269,10 +10264,10 @@
       <c r="L225" s="4"/>
     </row>
     <row r="226" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A226" s="101" t="s">
+      <c r="A226" s="99" t="s">
         <v>507</v>
       </c>
-      <c r="B226" s="101" t="s">
+      <c r="B226" s="99" t="s">
         <v>486</v>
       </c>
       <c r="C226" s="4" t="s">
@@ -10303,10 +10298,10 @@
       <c r="L226" s="4"/>
     </row>
     <row r="227" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A227" s="101" t="s">
+      <c r="A227" s="99" t="s">
         <v>503</v>
       </c>
-      <c r="B227" s="101" t="s">
+      <c r="B227" s="99" t="s">
         <v>487</v>
       </c>
       <c r="C227" s="4" t="s">
@@ -10340,7 +10335,7 @@
       <c r="A228" s="5" t="s">
         <v>504</v>
       </c>
-      <c r="B228" s="99" t="s">
+      <c r="B228" s="97" t="s">
         <v>83</v>
       </c>
       <c r="C228" s="4" t="s">
@@ -10371,10 +10366,10 @@
       <c r="L228" s="4"/>
     </row>
     <row r="229" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A229" s="101" t="s">
+      <c r="A229" s="99" t="s">
         <v>508</v>
       </c>
-      <c r="B229" s="101" t="s">
+      <c r="B229" s="99" t="s">
         <v>84</v>
       </c>
       <c r="C229" s="4" t="s">
@@ -10405,10 +10400,10 @@
       <c r="L229" s="4"/>
     </row>
     <row r="230" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A230" s="102" t="s">
+      <c r="A230" s="100" t="s">
         <v>510</v>
       </c>
-      <c r="B230" s="102" t="s">
+      <c r="B230" s="100" t="s">
         <v>488</v>
       </c>
       <c r="C230" s="4" t="s">
@@ -10439,10 +10434,10 @@
       <c r="L230" s="4"/>
     </row>
     <row r="231" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A231" s="104" t="s">
+      <c r="A231" s="102" t="s">
         <v>511</v>
       </c>
-      <c r="B231" s="104" t="s">
+      <c r="B231" s="102" t="s">
         <v>85</v>
       </c>
       <c r="C231" s="4" t="s">
@@ -10473,10 +10468,10 @@
       <c r="L231" s="4"/>
     </row>
     <row r="232" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A232" s="103" t="s">
+      <c r="A232" s="101" t="s">
         <v>512</v>
       </c>
-      <c r="B232" s="103" t="s">
+      <c r="B232" s="101" t="s">
         <v>86</v>
       </c>
       <c r="C232" s="4" t="s">
@@ -10507,10 +10502,10 @@
       <c r="L232" s="4"/>
     </row>
     <row r="233" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A233" s="105" t="s">
+      <c r="A233" s="103" t="s">
         <v>513</v>
       </c>
-      <c r="B233" s="106" t="s">
+      <c r="B233" s="104" t="s">
         <v>489</v>
       </c>
       <c r="C233" s="4" t="s">
@@ -10541,10 +10536,10 @@
       <c r="L233" s="4"/>
     </row>
     <row r="234" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A234" s="107" t="s">
+      <c r="A234" s="105" t="s">
         <v>514</v>
       </c>
-      <c r="B234" s="107" t="s">
+      <c r="B234" s="105" t="s">
         <v>87</v>
       </c>
       <c r="C234" s="4" t="s">
@@ -10578,7 +10573,7 @@
       <c r="A235" s="5" t="s">
         <v>509</v>
       </c>
-      <c r="B235" s="100" t="s">
+      <c r="B235" s="98" t="s">
         <v>88</v>
       </c>
       <c r="C235" s="4" t="s">
@@ -10612,7 +10607,7 @@
       <c r="A236" s="5" t="s">
         <v>515</v>
       </c>
-      <c r="B236" s="108" t="s">
+      <c r="B236" s="106" t="s">
         <v>490</v>
       </c>
       <c r="C236" s="4" t="s">
@@ -10646,7 +10641,7 @@
       <c r="A237" s="5" t="s">
         <v>517</v>
       </c>
-      <c r="B237" s="110" t="s">
+      <c r="B237" s="108" t="s">
         <v>89</v>
       </c>
       <c r="C237" s="4" t="s">
@@ -10680,7 +10675,7 @@
       <c r="A238" s="5" t="s">
         <v>518</v>
       </c>
-      <c r="B238" s="111" t="s">
+      <c r="B238" s="109" t="s">
         <v>90</v>
       </c>
       <c r="C238" s="4" t="s">
@@ -10714,7 +10709,7 @@
       <c r="A239" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="B239" s="109" t="s">
+      <c r="B239" s="107" t="s">
         <v>91</v>
       </c>
       <c r="C239" s="4" t="s">
@@ -10748,7 +10743,7 @@
       <c r="A240" s="5" t="s">
         <v>520</v>
       </c>
-      <c r="B240" s="112" t="s">
+      <c r="B240" s="110" t="s">
         <v>519</v>
       </c>
       <c r="C240" s="4" t="s">
@@ -10782,7 +10777,7 @@
       <c r="A241" s="5" t="s">
         <v>521</v>
       </c>
-      <c r="B241" s="113" t="s">
+      <c r="B241" s="111" t="s">
         <v>92</v>
       </c>
       <c r="C241" s="4" t="s">
@@ -10816,7 +10811,7 @@
       <c r="A242" s="5" t="s">
         <v>533</v>
       </c>
-      <c r="B242" s="116" t="s">
+      <c r="B242" s="114" t="s">
         <v>93</v>
       </c>
       <c r="C242" s="4" t="s">
@@ -10850,7 +10845,7 @@
       <c r="A243" s="5" t="s">
         <v>532</v>
       </c>
-      <c r="B243" s="115" t="s">
+      <c r="B243" s="113" t="s">
         <v>524</v>
       </c>
       <c r="C243" s="4" t="s">
@@ -10884,7 +10879,7 @@
       <c r="A244" s="5" t="s">
         <v>523</v>
       </c>
-      <c r="B244" s="114" t="s">
+      <c r="B244" s="112" t="s">
         <v>522</v>
       </c>
       <c r="C244" s="4" t="s">
@@ -10918,7 +10913,7 @@
       <c r="A245" s="5" t="s">
         <v>535</v>
       </c>
-      <c r="B245" s="117" t="s">
+      <c r="B245" s="115" t="s">
         <v>94</v>
       </c>
       <c r="C245" s="4" t="s">
@@ -10952,7 +10947,7 @@
       <c r="A246" s="5" t="s">
         <v>534</v>
       </c>
-      <c r="B246" s="118" t="s">
+      <c r="B246" s="116" t="s">
         <v>525</v>
       </c>
       <c r="C246" s="4" t="s">
@@ -10986,7 +10981,7 @@
       <c r="A247" s="5" t="s">
         <v>536</v>
       </c>
-      <c r="B247" s="119" t="s">
+      <c r="B247" s="117" t="s">
         <v>96</v>
       </c>
       <c r="C247" s="4" t="s">
@@ -11014,13 +11009,13 @@
         <v>135</v>
       </c>
       <c r="K247" s="4"/>
-      <c r="L247" s="10"/>
+      <c r="L247" s="9"/>
     </row>
     <row r="248" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A248" s="5" t="s">
         <v>537</v>
       </c>
-      <c r="B248" s="120" t="s">
+      <c r="B248" s="118" t="s">
         <v>526</v>
       </c>
       <c r="C248" s="4" t="s">
@@ -11054,7 +11049,7 @@
       <c r="A249" s="5" t="s">
         <v>538</v>
       </c>
-      <c r="B249" s="121" t="s">
+      <c r="B249" s="119" t="s">
         <v>97</v>
       </c>
       <c r="C249" s="4" t="s">
@@ -11088,7 +11083,7 @@
       <c r="A250" s="5" t="s">
         <v>539</v>
       </c>
-      <c r="B250" s="122" t="s">
+      <c r="B250" s="120" t="s">
         <v>527</v>
       </c>
       <c r="C250" s="4" t="s">
@@ -11122,7 +11117,7 @@
       <c r="A251" s="5" t="s">
         <v>543</v>
       </c>
-      <c r="B251" s="126" t="s">
+      <c r="B251" s="124" t="s">
         <v>528</v>
       </c>
       <c r="C251" s="4" t="s">
@@ -11153,10 +11148,10 @@
       <c r="L251" s="4"/>
     </row>
     <row r="252" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A252" s="124" t="s">
+      <c r="A252" s="122" t="s">
         <v>541</v>
       </c>
-      <c r="B252" s="125" t="s">
+      <c r="B252" s="123" t="s">
         <v>529</v>
       </c>
       <c r="C252" s="4" t="s">
@@ -11190,7 +11185,7 @@
       <c r="A253" s="5" t="s">
         <v>540</v>
       </c>
-      <c r="B253" s="123" t="s">
+      <c r="B253" s="121" t="s">
         <v>530</v>
       </c>
       <c r="C253" s="4" t="s">
@@ -11224,7 +11219,7 @@
       <c r="A254" s="5" t="s">
         <v>542</v>
       </c>
-      <c r="B254" s="124" t="s">
+      <c r="B254" s="122" t="s">
         <v>100</v>
       </c>
       <c r="C254" s="4" t="s">
@@ -11258,7 +11253,7 @@
       <c r="A255" s="5" t="s">
         <v>546</v>
       </c>
-      <c r="B255" s="128" t="s">
+      <c r="B255" s="126" t="s">
         <v>547</v>
       </c>
       <c r="C255" s="4" t="s">
@@ -11292,7 +11287,7 @@
       <c r="A256" s="5" t="s">
         <v>551</v>
       </c>
-      <c r="B256" s="129" t="s">
+      <c r="B256" s="127" t="s">
         <v>531</v>
       </c>
       <c r="C256" s="4" t="s">
@@ -11326,7 +11321,7 @@
       <c r="A257" s="5" t="s">
         <v>544</v>
       </c>
-      <c r="B257" s="128" t="s">
+      <c r="B257" s="126" t="s">
         <v>545</v>
       </c>
       <c r="C257" s="4" t="s">
@@ -11357,10 +11352,10 @@
       <c r="L257" s="4"/>
     </row>
     <row r="258" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A258" s="128" t="s">
+      <c r="A258" s="126" t="s">
         <v>548</v>
       </c>
-      <c r="B258" s="127" t="s">
+      <c r="B258" s="125" t="s">
         <v>102</v>
       </c>
       <c r="C258" s="4" t="s">
@@ -11391,10 +11386,10 @@
       <c r="L258" s="4"/>
     </row>
     <row r="259" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A259" s="128" t="s">
+      <c r="A259" s="126" t="s">
         <v>550</v>
       </c>
-      <c r="B259" s="128" t="s">
+      <c r="B259" s="126" t="s">
         <v>549</v>
       </c>
       <c r="C259" s="4" t="s">
@@ -11424,45 +11419,45 @@
       <c r="K259" s="4"/>
       <c r="L259" s="4"/>
     </row>
-    <row r="260" spans="1:12" s="199" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A260" s="200" t="s">
+    <row r="260" spans="1:12" s="197" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A260" s="198" t="s">
         <v>653</v>
       </c>
-      <c r="B260" s="200" t="s">
+      <c r="B260" s="198" t="s">
         <v>101</v>
       </c>
-      <c r="C260" s="202" t="s">
-        <v>3</v>
-      </c>
-      <c r="D260" s="202">
+      <c r="C260" s="200" t="s">
+        <v>3</v>
+      </c>
+      <c r="D260" s="200">
         <v>2014</v>
       </c>
-      <c r="E260" s="202">
-        <v>3</v>
-      </c>
-      <c r="F260" s="202">
-        <v>0</v>
-      </c>
-      <c r="G260" s="202">
-        <v>0</v>
-      </c>
-      <c r="H260" s="202">
-        <v>0</v>
-      </c>
-      <c r="I260" s="202">
-        <v>0</v>
-      </c>
-      <c r="J260" s="202" t="s">
-        <v>135</v>
-      </c>
-      <c r="K260" s="202"/>
-      <c r="L260" s="202"/>
+      <c r="E260" s="200">
+        <v>3</v>
+      </c>
+      <c r="F260" s="200">
+        <v>0</v>
+      </c>
+      <c r="G260" s="200">
+        <v>0</v>
+      </c>
+      <c r="H260" s="200">
+        <v>0</v>
+      </c>
+      <c r="I260" s="200">
+        <v>0</v>
+      </c>
+      <c r="J260" s="200" t="s">
+        <v>135</v>
+      </c>
+      <c r="K260" s="200"/>
+      <c r="L260" s="200"/>
     </row>
     <row r="261" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A261" s="133" t="s">
+      <c r="A261" s="131" t="s">
         <v>561</v>
       </c>
-      <c r="B261" s="133" t="s">
+      <c r="B261" s="131" t="s">
         <v>560</v>
       </c>
       <c r="C261" s="4" t="s">
@@ -11493,10 +11488,10 @@
       <c r="L261" s="4"/>
     </row>
     <row r="262" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A262" s="130" t="s">
+      <c r="A262" s="128" t="s">
         <v>558</v>
       </c>
-      <c r="B262" s="131" t="s">
+      <c r="B262" s="129" t="s">
         <v>552</v>
       </c>
       <c r="C262" s="4" t="s">
@@ -11524,13 +11519,13 @@
         <v>135</v>
       </c>
       <c r="K262" s="4"/>
-      <c r="L262" s="7"/>
+      <c r="L262" s="6"/>
     </row>
     <row r="263" spans="1:12" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A263" s="5" t="s">
         <v>559</v>
       </c>
-      <c r="B263" s="132" t="s">
+      <c r="B263" s="130" t="s">
         <v>562</v>
       </c>
       <c r="C263" s="4" t="s">
@@ -11558,13 +11553,13 @@
         <v>135</v>
       </c>
       <c r="K263" s="4"/>
-      <c r="L263" s="11"/>
+      <c r="L263" s="10"/>
     </row>
     <row r="264" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A264" s="5" t="s">
         <v>565</v>
       </c>
-      <c r="B264" s="135" t="s">
+      <c r="B264" s="133" t="s">
         <v>105</v>
       </c>
       <c r="C264" s="4" t="s">
@@ -11595,10 +11590,10 @@
       <c r="L264" s="4"/>
     </row>
     <row r="265" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A265" s="137" t="s">
+      <c r="A265" s="135" t="s">
         <v>570</v>
       </c>
-      <c r="B265" s="137" t="s">
+      <c r="B265" s="135" t="s">
         <v>569</v>
       </c>
       <c r="C265" s="4" t="s">
@@ -11632,7 +11627,7 @@
       <c r="A266" s="5" t="s">
         <v>564</v>
       </c>
-      <c r="B266" s="134" t="s">
+      <c r="B266" s="132" t="s">
         <v>553</v>
       </c>
       <c r="C266" s="4" t="s">
@@ -11666,7 +11661,7 @@
       <c r="A267" s="5" t="s">
         <v>568</v>
       </c>
-      <c r="B267" s="137" t="s">
+      <c r="B267" s="135" t="s">
         <v>106</v>
       </c>
       <c r="C267" s="4" t="s">
@@ -11700,7 +11695,7 @@
       <c r="A268" s="5" t="s">
         <v>566</v>
       </c>
-      <c r="B268" s="136" t="s">
+      <c r="B268" s="134" t="s">
         <v>554</v>
       </c>
       <c r="C268" s="4" t="s">
@@ -11734,7 +11729,7 @@
       <c r="A269" s="5" t="s">
         <v>567</v>
       </c>
-      <c r="B269" s="138" t="s">
+      <c r="B269" s="136" t="s">
         <v>107</v>
       </c>
       <c r="C269" s="4" t="s">
@@ -11768,7 +11763,7 @@
       <c r="A270" s="5" t="s">
         <v>571</v>
       </c>
-      <c r="B270" s="139" t="s">
+      <c r="B270" s="137" t="s">
         <v>108</v>
       </c>
       <c r="C270" s="4" t="s">
@@ -11802,7 +11797,7 @@
       <c r="A271" s="5" t="s">
         <v>574</v>
       </c>
-      <c r="B271" s="141" t="s">
+      <c r="B271" s="139" t="s">
         <v>555</v>
       </c>
       <c r="C271" s="4" t="s">
@@ -11836,7 +11831,7 @@
       <c r="A272" s="5" t="s">
         <v>573</v>
       </c>
-      <c r="B272" s="140" t="s">
+      <c r="B272" s="138" t="s">
         <v>572</v>
       </c>
       <c r="C272" s="4" t="s">
@@ -11870,7 +11865,7 @@
       <c r="A273" s="5" t="s">
         <v>575</v>
       </c>
-      <c r="B273" s="142" t="s">
+      <c r="B273" s="140" t="s">
         <v>109</v>
       </c>
       <c r="C273" s="4" t="s">
@@ -11904,7 +11899,7 @@
       <c r="A274" s="5" t="s">
         <v>578</v>
       </c>
-      <c r="B274" s="145" t="s">
+      <c r="B274" s="143" t="s">
         <v>577</v>
       </c>
       <c r="C274" s="4" t="s">
@@ -11935,10 +11930,10 @@
       <c r="L274" s="4"/>
     </row>
     <row r="275" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A275" s="143" t="s">
+      <c r="A275" s="141" t="s">
         <v>576</v>
       </c>
-      <c r="B275" s="144" t="s">
+      <c r="B275" s="142" t="s">
         <v>556</v>
       </c>
       <c r="C275" s="4" t="s">
@@ -11972,7 +11967,7 @@
       <c r="A276" s="5" t="s">
         <v>580</v>
       </c>
-      <c r="B276" s="146" t="s">
+      <c r="B276" s="144" t="s">
         <v>579</v>
       </c>
       <c r="C276" s="4" t="s">
@@ -12003,10 +11998,10 @@
       <c r="L276" s="4"/>
     </row>
     <row r="277" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A277" s="148" t="s">
+      <c r="A277" s="146" t="s">
         <v>582</v>
       </c>
-      <c r="B277" s="149" t="s">
+      <c r="B277" s="147" t="s">
         <v>557</v>
       </c>
       <c r="C277" s="4" t="s">
@@ -12040,7 +12035,7 @@
       <c r="A278" s="5" t="s">
         <v>584</v>
       </c>
-      <c r="B278" s="152" t="s">
+      <c r="B278" s="150" t="s">
         <v>585</v>
       </c>
       <c r="C278" s="4" t="s">
@@ -12071,10 +12066,10 @@
       <c r="L278" s="4"/>
     </row>
     <row r="279" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A279" s="150" t="s">
+      <c r="A279" s="148" t="s">
         <v>583</v>
       </c>
-      <c r="B279" s="151" t="s">
+      <c r="B279" s="149" t="s">
         <v>563</v>
       </c>
       <c r="C279" s="4" t="s">
@@ -12108,7 +12103,7 @@
       <c r="A280" s="5" t="s">
         <v>581</v>
       </c>
-      <c r="B280" s="147" t="s">
+      <c r="B280" s="145" t="s">
         <v>110</v>
       </c>
       <c r="C280" s="4" t="s">
@@ -12139,10 +12134,10 @@
       <c r="L280" s="4"/>
     </row>
     <row r="281" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A281" s="158" t="s">
+      <c r="A281" s="156" t="s">
         <v>596</v>
       </c>
-      <c r="B281" s="159" t="s">
+      <c r="B281" s="157" t="s">
         <v>597</v>
       </c>
       <c r="C281" s="4" t="s">
@@ -12173,10 +12168,10 @@
       <c r="L281" s="4"/>
     </row>
     <row r="282" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A282" s="154" t="s">
+      <c r="A282" s="152" t="s">
         <v>594</v>
       </c>
-      <c r="B282" s="154" t="s">
+      <c r="B282" s="152" t="s">
         <v>111</v>
       </c>
       <c r="C282" s="4" t="s">
@@ -12210,7 +12205,7 @@
       <c r="A283" s="5" t="s">
         <v>592</v>
       </c>
-      <c r="B283" s="153" t="s">
+      <c r="B283" s="151" t="s">
         <v>586</v>
       </c>
       <c r="C283" s="4" t="s">
@@ -12241,10 +12236,10 @@
       <c r="L283" s="4"/>
     </row>
     <row r="284" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A284" s="154" t="s">
+      <c r="A284" s="152" t="s">
         <v>593</v>
       </c>
-      <c r="B284" s="155" t="s">
+      <c r="B284" s="153" t="s">
         <v>112</v>
       </c>
       <c r="C284" s="4" t="s">
@@ -12275,10 +12270,10 @@
       <c r="L284" s="4"/>
     </row>
     <row r="285" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A285" s="156" t="s">
+      <c r="A285" s="154" t="s">
         <v>595</v>
       </c>
-      <c r="B285" s="157" t="s">
+      <c r="B285" s="155" t="s">
         <v>587</v>
       </c>
       <c r="C285" s="4" t="s">
@@ -12309,10 +12304,10 @@
       <c r="L285" s="4"/>
     </row>
     <row r="286" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A286" s="158" t="s">
+      <c r="A286" s="156" t="s">
         <v>598</v>
       </c>
-      <c r="B286" s="158" t="s">
+      <c r="B286" s="156" t="s">
         <v>113</v>
       </c>
       <c r="C286" s="4" t="s">
@@ -12343,10 +12338,10 @@
       <c r="L286" s="4"/>
     </row>
     <row r="287" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A287" s="162" t="s">
+      <c r="A287" s="160" t="s">
         <v>600</v>
       </c>
-      <c r="B287" s="163" t="s">
+      <c r="B287" s="161" t="s">
         <v>114</v>
       </c>
       <c r="C287" s="4" t="s">
@@ -12377,10 +12372,10 @@
       <c r="L287" s="4"/>
     </row>
     <row r="288" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A288" s="164" t="s">
+      <c r="A288" s="162" t="s">
         <v>602</v>
       </c>
-      <c r="B288" s="165" t="s">
+      <c r="B288" s="163" t="s">
         <v>601</v>
       </c>
       <c r="C288" s="4" t="s">
@@ -12411,10 +12406,10 @@
       <c r="L288" s="4"/>
     </row>
     <row r="289" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A289" s="160" t="s">
+      <c r="A289" s="158" t="s">
         <v>599</v>
       </c>
-      <c r="B289" s="161" t="s">
+      <c r="B289" s="159" t="s">
         <v>588</v>
       </c>
       <c r="C289" s="4" t="s">
@@ -12445,10 +12440,10 @@
       <c r="L289" s="4"/>
     </row>
     <row r="290" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A290" s="166" t="s">
+      <c r="A290" s="164" t="s">
         <v>603</v>
       </c>
-      <c r="B290" s="167" t="s">
+      <c r="B290" s="165" t="s">
         <v>589</v>
       </c>
       <c r="C290" s="4" t="s">
@@ -12479,10 +12474,10 @@
       <c r="L290" s="4"/>
     </row>
     <row r="291" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A291" s="170" t="s">
+      <c r="A291" s="168" t="s">
         <v>605</v>
       </c>
-      <c r="B291" s="171" t="s">
+      <c r="B291" s="169" t="s">
         <v>590</v>
       </c>
       <c r="C291" s="4" t="s">
@@ -12513,10 +12508,10 @@
       <c r="L291" s="4"/>
     </row>
     <row r="292" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A292" s="168" t="s">
+      <c r="A292" s="166" t="s">
         <v>604</v>
       </c>
-      <c r="B292" s="169" t="s">
+      <c r="B292" s="167" t="s">
         <v>591</v>
       </c>
       <c r="C292" s="4" t="s">
@@ -12547,10 +12542,10 @@
       <c r="L292" s="4"/>
     </row>
     <row r="293" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A293" s="172" t="s">
+      <c r="A293" s="170" t="s">
         <v>606</v>
       </c>
-      <c r="B293" s="173" t="s">
+      <c r="B293" s="171" t="s">
         <v>115</v>
       </c>
       <c r="C293" s="4" t="s">
@@ -12581,10 +12576,10 @@
       <c r="L293" s="4"/>
     </row>
     <row r="294" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A294" s="174" t="s">
+      <c r="A294" s="172" t="s">
         <v>610</v>
       </c>
-      <c r="B294" s="175" t="s">
+      <c r="B294" s="173" t="s">
         <v>116</v>
       </c>
       <c r="C294" s="4" t="s">
@@ -12615,10 +12610,10 @@
       <c r="L294" s="4"/>
     </row>
     <row r="295" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A295" s="175" t="s">
+      <c r="A295" s="173" t="s">
         <v>609</v>
       </c>
-      <c r="B295" s="175" t="s">
+      <c r="B295" s="173" t="s">
         <v>117</v>
       </c>
       <c r="C295" s="4" t="s">
@@ -12649,10 +12644,10 @@
       <c r="L295" s="4"/>
     </row>
     <row r="296" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A296" s="175" t="s">
+      <c r="A296" s="173" t="s">
         <v>607</v>
       </c>
-      <c r="B296" s="175" t="s">
+      <c r="B296" s="173" t="s">
         <v>608</v>
       </c>
       <c r="C296" s="4" t="s">
@@ -12683,10 +12678,10 @@
       <c r="L296" s="4"/>
     </row>
     <row r="297" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A297" s="175" t="s">
+      <c r="A297" s="173" t="s">
         <v>616</v>
       </c>
-      <c r="B297" s="175" t="s">
+      <c r="B297" s="173" t="s">
         <v>615</v>
       </c>
       <c r="C297" s="4" t="s">
@@ -12717,10 +12712,10 @@
       <c r="L297" s="4"/>
     </row>
     <row r="298" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A298" s="175" t="s">
+      <c r="A298" s="173" t="s">
         <v>613</v>
       </c>
-      <c r="B298" s="175" t="s">
+      <c r="B298" s="173" t="s">
         <v>612</v>
       </c>
       <c r="C298" s="4" t="s">
@@ -12751,10 +12746,10 @@
       <c r="L298" s="4"/>
     </row>
     <row r="299" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A299" s="175" t="s">
+      <c r="A299" s="173" t="s">
         <v>611</v>
       </c>
-      <c r="B299" s="175" t="s">
+      <c r="B299" s="173" t="s">
         <v>118</v>
       </c>
       <c r="C299" s="4" t="s">
@@ -12785,10 +12780,10 @@
       <c r="L299" s="4"/>
     </row>
     <row r="300" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A300" s="175" t="s">
+      <c r="A300" s="173" t="s">
         <v>614</v>
       </c>
-      <c r="B300" s="175" t="s">
+      <c r="B300" s="173" t="s">
         <v>119</v>
       </c>
       <c r="C300" s="4" t="s">
@@ -12819,10 +12814,10 @@
       <c r="L300" s="4"/>
     </row>
     <row r="301" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A301" s="175" t="s">
+      <c r="A301" s="173" t="s">
         <v>620</v>
       </c>
-      <c r="B301" s="175" t="s">
+      <c r="B301" s="173" t="s">
         <v>621</v>
       </c>
       <c r="C301" s="4" t="s">
@@ -12853,10 +12848,10 @@
       <c r="L301" s="4"/>
     </row>
     <row r="302" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A302" s="175" t="s">
+      <c r="A302" s="173" t="s">
         <v>622</v>
       </c>
-      <c r="B302" s="175" t="s">
+      <c r="B302" s="173" t="s">
         <v>120</v>
       </c>
       <c r="C302" s="4" t="s">
@@ -12887,10 +12882,10 @@
       <c r="L302" s="4"/>
     </row>
     <row r="303" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A303" s="175" t="s">
+      <c r="A303" s="173" t="s">
         <v>618</v>
       </c>
-      <c r="B303" s="175" t="s">
+      <c r="B303" s="173" t="s">
         <v>619</v>
       </c>
       <c r="C303" s="4" t="s">
@@ -12920,45 +12915,46 @@
       <c r="K303" s="4"/>
       <c r="L303" s="4"/>
     </row>
-    <row r="304" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A304" s="175" t="s">
+    <row r="304" spans="1:12" s="200" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A304" s="200" t="s">
         <v>617</v>
       </c>
-      <c r="B304" s="175" t="s">
+      <c r="B304" s="200" t="s">
         <v>121</v>
       </c>
-      <c r="C304" s="4" t="s">
+      <c r="C304" s="200" t="s">
         <v>36</v>
       </c>
-      <c r="D304" s="4">
+      <c r="D304" s="200">
         <v>2014</v>
       </c>
-      <c r="E304" s="4">
-        <v>1</v>
-      </c>
-      <c r="F304" s="4">
-        <v>1</v>
-      </c>
-      <c r="G304" s="4">
-        <v>1</v>
-      </c>
-      <c r="H304" s="4">
-        <v>0</v>
-      </c>
-      <c r="I304" s="4">
-        <v>0</v>
-      </c>
-      <c r="J304" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="K304" s="4"/>
-      <c r="L304" s="4"/>
+      <c r="E304" s="200">
+        <v>1</v>
+      </c>
+      <c r="F304" s="200">
+        <v>1</v>
+      </c>
+      <c r="G304" s="200">
+        <v>1</v>
+      </c>
+      <c r="H304" s="200">
+        <v>0</v>
+      </c>
+      <c r="I304" s="200">
+        <v>0</v>
+      </c>
+      <c r="J304" s="200" t="s">
+        <v>135</v>
+      </c>
+      <c r="K304" s="200" t="s">
+        <v>656</v>
+      </c>
     </row>
     <row r="305" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A305" s="175" t="s">
+      <c r="A305" s="173" t="s">
         <v>623</v>
       </c>
-      <c r="B305" s="175" t="s">
+      <c r="B305" s="173" t="s">
         <v>122</v>
       </c>
       <c r="C305" s="4" t="s">
@@ -12989,10 +12985,10 @@
       <c r="L305" s="4"/>
     </row>
     <row r="306" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A306" s="175" t="s">
+      <c r="A306" s="173" t="s">
         <v>625</v>
       </c>
-      <c r="B306" s="175" t="s">
+      <c r="B306" s="173" t="s">
         <v>624</v>
       </c>
       <c r="C306" s="4" t="s">
@@ -13023,10 +13019,10 @@
       <c r="L306" s="4"/>
     </row>
     <row r="307" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A307" s="175" t="s">
+      <c r="A307" s="173" t="s">
         <v>637</v>
       </c>
-      <c r="B307" s="183" t="s">
+      <c r="B307" s="181" t="s">
         <v>635</v>
       </c>
       <c r="C307" s="4" t="s">
@@ -13057,10 +13053,10 @@
       <c r="L307" s="4"/>
     </row>
     <row r="308" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A308" s="184" t="s">
+      <c r="A308" s="182" t="s">
         <v>638</v>
       </c>
-      <c r="B308" s="184" t="s">
+      <c r="B308" s="182" t="s">
         <v>636</v>
       </c>
       <c r="C308" s="4" t="s">
@@ -13091,10 +13087,10 @@
       <c r="L308" s="4"/>
     </row>
     <row r="309" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A309" s="179" t="s">
+      <c r="A309" s="177" t="s">
         <v>633</v>
       </c>
-      <c r="B309" s="180" t="s">
+      <c r="B309" s="178" t="s">
         <v>627</v>
       </c>
       <c r="C309" s="4" t="s">
@@ -13125,10 +13121,10 @@
       <c r="L309" s="4"/>
     </row>
     <row r="310" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A310" s="187" t="s">
+      <c r="A310" s="185" t="s">
         <v>640</v>
       </c>
-      <c r="B310" s="188" t="s">
+      <c r="B310" s="186" t="s">
         <v>628</v>
       </c>
       <c r="C310" s="4" t="s">
@@ -13159,10 +13155,10 @@
       <c r="L310" s="4"/>
     </row>
     <row r="311" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A311" s="185" t="s">
+      <c r="A311" s="183" t="s">
         <v>639</v>
       </c>
-      <c r="B311" s="186" t="s">
+      <c r="B311" s="184" t="s">
         <v>629</v>
       </c>
       <c r="C311" s="4" t="s">
@@ -13193,10 +13189,10 @@
       <c r="L311" s="4"/>
     </row>
     <row r="312" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A312" s="181" t="s">
+      <c r="A312" s="179" t="s">
         <v>634</v>
       </c>
-      <c r="B312" s="182" t="s">
+      <c r="B312" s="180" t="s">
         <v>630</v>
       </c>
       <c r="C312" s="4" t="s">
@@ -13227,10 +13223,10 @@
       <c r="L312" s="4"/>
     </row>
     <row r="313" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A313" s="177" t="s">
+      <c r="A313" s="175" t="s">
         <v>626</v>
       </c>
-      <c r="B313" s="178" t="s">
+      <c r="B313" s="176" t="s">
         <v>123</v>
       </c>
       <c r="C313" s="4" t="s">
@@ -13261,10 +13257,10 @@
       <c r="L313" s="4"/>
     </row>
     <row r="314" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A314" s="187" t="s">
+      <c r="A314" s="185" t="s">
         <v>642</v>
       </c>
-      <c r="B314" s="187" t="s">
+      <c r="B314" s="185" t="s">
         <v>124</v>
       </c>
       <c r="C314" s="4" t="s">
@@ -13295,10 +13291,10 @@
       <c r="L314" s="4"/>
     </row>
     <row r="315" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A315" s="187" t="s">
+      <c r="A315" s="185" t="s">
         <v>641</v>
       </c>
-      <c r="B315" s="187" t="s">
+      <c r="B315" s="185" t="s">
         <v>125</v>
       </c>
       <c r="C315" s="4" t="s">
@@ -13329,10 +13325,10 @@
       <c r="L315" s="4"/>
     </row>
     <row r="316" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A316" s="191" t="s">
+      <c r="A316" s="189" t="s">
         <v>644</v>
       </c>
-      <c r="B316" s="192" t="s">
+      <c r="B316" s="190" t="s">
         <v>126</v>
       </c>
       <c r="C316" s="4" t="s">
@@ -13363,7 +13359,7 @@
       <c r="L316" s="4"/>
     </row>
     <row r="317" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A317" s="191" t="s">
+      <c r="A317" s="189" t="s">
         <v>645</v>
       </c>
       <c r="B317" s="5" t="s">
@@ -13397,10 +13393,10 @@
       <c r="L317" s="4"/>
     </row>
     <row r="318" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A318" s="189" t="s">
+      <c r="A318" s="187" t="s">
         <v>643</v>
       </c>
-      <c r="B318" s="190" t="s">
+      <c r="B318" s="188" t="s">
         <v>127</v>
       </c>
       <c r="C318" s="4" t="s">
@@ -13431,10 +13427,10 @@
       <c r="L318" s="4"/>
     </row>
     <row r="319" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A319" s="197" t="s">
+      <c r="A319" s="195" t="s">
         <v>652</v>
       </c>
-      <c r="B319" s="197" t="s">
+      <c r="B319" s="195" t="s">
         <v>128</v>
       </c>
       <c r="C319" s="4" t="s">
@@ -13465,10 +13461,10 @@
       <c r="L319" s="4"/>
     </row>
     <row r="320" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A320" s="193" t="s">
+      <c r="A320" s="191" t="s">
         <v>647</v>
       </c>
-      <c r="B320" s="194" t="s">
+      <c r="B320" s="192" t="s">
         <v>631</v>
       </c>
       <c r="C320" s="4" t="s">
@@ -13499,10 +13495,10 @@
       <c r="L320" s="4"/>
     </row>
     <row r="321" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A321" s="197" t="s">
+      <c r="A321" s="195" t="s">
         <v>650</v>
       </c>
-      <c r="B321" s="176" t="s">
+      <c r="B321" s="174" t="s">
         <v>651</v>
       </c>
       <c r="C321" s="4" t="s">
@@ -13533,10 +13529,10 @@
       <c r="L321" s="4"/>
     </row>
     <row r="322" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A322" s="197" t="s">
+      <c r="A322" s="195" t="s">
         <v>649</v>
       </c>
-      <c r="B322" s="198" t="s">
+      <c r="B322" s="196" t="s">
         <v>632</v>
       </c>
       <c r="C322" s="4" t="s">
@@ -13567,10 +13563,10 @@
       <c r="L322" s="4"/>
     </row>
     <row r="323" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A323" s="195" t="s">
+      <c r="A323" s="193" t="s">
         <v>648</v>
       </c>
-      <c r="B323" s="196" t="s">
+      <c r="B323" s="194" t="s">
         <v>129</v>
       </c>
       <c r="C323" s="4" t="s">

</xml_diff>

<commit_message>
adapting code file to includes flowchart, edit Hyp and inclusion_Hyp, adding READme for code file
</commit_message>
<xml_diff>
--- a/Data sets/Hyp/inclusion_Hyp.xlsx
+++ b/Data sets/Hyp/inclusion_Hyp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EliseSchramkowski\Documents\GitHub\thesis\Data sets\Hyp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241932ED-6BDB-47E1-ACFA-F0B1A2DB9C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A25D738-15B1-4B11-A35B-1D14FE72FE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13512" yWindow="2952" windowWidth="15120" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15552" yWindow="288" windowWidth="15120" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Articles" sheetId="1" r:id="rId1"/>
@@ -2676,8 +2676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M325"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A290" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="A304" sqref="A304:XFD304"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="G94" sqref="G94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12935,7 +12935,7 @@
         <v>1</v>
       </c>
       <c r="G304" s="200">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H304" s="200">
         <v>0</v>

</xml_diff>